<commit_message>
reporte caso del mes
</commit_message>
<xml_diff>
--- a/public_html/admin/export_to_excel.xlsx
+++ b/public_html/admin/export_to_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Forum Leader</t>
   </si>
@@ -87,6 +87,21 @@
   </si>
   <si>
     <t>Mauricio Marchese</t>
+  </si>
+  <si>
+    <t>2017-06-20 08:00:00</t>
+  </si>
+  <si>
+    <t>2017-06-20 13:00:00</t>
+  </si>
+  <si>
+    <t>2017-06-15 13:00:00</t>
+  </si>
+  <si>
+    <t>xcvzxcv</t>
+  </si>
+  <si>
+    <t>Tom</t>
   </si>
 </sst>
 </file>
@@ -425,7 +440,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,6 +578,60 @@
         <v>23</v>
       </c>
       <c r="J5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>223</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>223</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>